<commit_message>
added userdir in excelreader
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -165,55 +165,55 @@
     <t>StageProbabilityProbability</t>
   </si>
   <si>
+    <t>Vijay1234</t>
+  </si>
+  <si>
+    <t>Budget Price</t>
+  </si>
+  <si>
+    <t>Automation Test Description</t>
+  </si>
+  <si>
+    <t>5f</t>
+  </si>
+  <si>
+    <t>2f</t>
+  </si>
+  <si>
+    <t>06114080</t>
+  </si>
+  <si>
+    <t>KOFCOL TRB 201</t>
+  </si>
+  <si>
+    <t>AU21 - Sydney Region</t>
+  </si>
+  <si>
+    <t>AU22 - Newcastle Region</t>
+  </si>
+  <si>
+    <t>AustraliaRopes_For Automation</t>
+  </si>
+  <si>
+    <t>07006025</t>
+  </si>
+  <si>
+    <t>Montréal</t>
+  </si>
+  <si>
+    <t>Québec City</t>
+  </si>
+  <si>
+    <t>SeismicArea</t>
+  </si>
+  <si>
+    <t>WeeklyTeamCostforZone</t>
+  </si>
+  <si>
+    <t>WeeklyTeamCostforRoomandBoard</t>
+  </si>
+  <si>
     <t>s.vijay@kone.com.qa</t>
-  </si>
-  <si>
-    <t>Vijay1234</t>
-  </si>
-  <si>
-    <t>Budget Price</t>
-  </si>
-  <si>
-    <t>Automation Test Description</t>
-  </si>
-  <si>
-    <t>5f</t>
-  </si>
-  <si>
-    <t>2f</t>
-  </si>
-  <si>
-    <t>06114080</t>
-  </si>
-  <si>
-    <t>KOFCOL TRB 201</t>
-  </si>
-  <si>
-    <t>AU21 - Sydney Region</t>
-  </si>
-  <si>
-    <t>AU22 - Newcastle Region</t>
-  </si>
-  <si>
-    <t>AustraliaRopes_For Automation</t>
-  </si>
-  <si>
-    <t>07006025</t>
-  </si>
-  <si>
-    <t>Montréal</t>
-  </si>
-  <si>
-    <t>Québec City</t>
-  </si>
-  <si>
-    <t>SeismicArea</t>
-  </si>
-  <si>
-    <t>WeeklyTeamCostforZone</t>
-  </si>
-  <si>
-    <t>WeeklyTeamCostforRoomandBoard</t>
   </si>
 </sst>
 </file>
@@ -621,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -740,7 +740,7 @@
         <v>3</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>11</v>
@@ -764,16 +764,16 @@
         <v>2001</v>
       </c>
       <c r="Q2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="S2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="U2" s="3">
         <v>22</v>
@@ -912,7 +912,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4">
         <v>1813</v>
@@ -927,10 +927,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="I2" s="4">
         <v>13012004</v>
@@ -939,7 +939,7 @@
         <v>11</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L2" s="4">
         <v>0</v>
@@ -957,16 +957,16 @@
         <v>2001</v>
       </c>
       <c r="Q2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="S2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="U2" s="3">
         <v>22</v>
@@ -1064,13 +1064,13 @@
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
@@ -1132,10 +1132,10 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="I2" s="4">
         <v>2</v>
@@ -1147,7 +1147,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>11</v>
@@ -1177,10 +1177,10 @@
         <v>41</v>
       </c>
       <c r="V2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="X2" s="3">
         <v>22</v>
@@ -1223,9 +1223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1251,10 +1249,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
added locators for new objects for canada in projectoverview
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -1008,7 +1008,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1223,7 +1225,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
including multiequipment add work-in-progress
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
   <si>
     <t>KOFCOL TRB SFA</t>
   </si>
@@ -211,6 +211,27 @@
   </si>
   <si>
     <t>Automation_CKEHydromod</t>
+  </si>
+  <si>
+    <t>EquipmentID_2</t>
+  </si>
+  <si>
+    <t>TemplateName2</t>
+  </si>
+  <si>
+    <t>Automation_Template_forEscalator</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>Automation_GroupName</t>
+  </si>
+  <si>
+    <t>EquipmentinService_Escalator</t>
+  </si>
+  <si>
+    <t>EIS Escalator</t>
   </si>
 </sst>
 </file>
@@ -616,11 +637,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -628,27 +647,31 @@
     <col min="2" max="2" width="13.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.6328125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="6.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.7265625" style="5"/>
+    <col min="5" max="5" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.08984375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6328125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="6.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -662,58 +685,70 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -726,55 +761,67 @@
       <c r="D2" s="4">
         <v>10503512</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="4">
+        <v>11234846</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="4">
+      <c r="N2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="4">
         <v>0</v>
       </c>
-      <c r="M2" s="4">
+      <c r="Q2" s="4">
         <v>3</v>
       </c>
-      <c r="N2" s="4">
+      <c r="R2" s="4">
         <v>6</v>
       </c>
-      <c r="O2" s="4">
+      <c r="S2" s="4">
         <v>10</v>
       </c>
-      <c r="P2" s="4">
+      <c r="T2" s="4">
         <v>2001</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="3">
+      <c r="Y2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -782,7 +829,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I2" numberStoredAsText="1"/>
+    <ignoredError sqref="J2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -803,7 +850,7 @@
           <x14:formula1>
             <xm:f>'-na-'!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
+          <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1225,7 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
partially including data retriving from fullgrid
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
   <si>
     <t>KOFCOL TRB SFA</t>
   </si>
@@ -232,9 +232,6 @@
   </si>
   <si>
     <t>EIS Escalator</t>
-  </si>
-  <si>
-    <t>4f</t>
   </si>
   <si>
     <t>changeRegionalDiscount</t>
@@ -706,7 +703,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -775,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -811,19 +810,19 @@
         <v>23</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>39</v>
@@ -867,7 +866,7 @@
         <v>47</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>9</v>
@@ -900,22 +899,22 @@
         <v>2001</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>43</v>
@@ -1031,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -1067,19 +1066,19 @@
         <v>23</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>39</v>
@@ -1123,7 +1122,7 @@
         <v>13012004</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>9</v>
@@ -1156,22 +1155,22 @@
         <v>2001</v>
       </c>
       <c r="V2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AA2" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>43</v>
@@ -1220,7 +1219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1298,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>17</v>
@@ -1334,19 +1333,19 @@
         <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>39</v>
@@ -1399,7 +1398,7 @@
         <v>52</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>9</v>
@@ -1435,19 +1434,19 @@
         <v>45</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AB2" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD2" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="AD2" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
partially updating ctrl+a actionitem_1 Entering 'First Maintenance' price if not available
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestMethods/src/com/KTOC/TRB/testautomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="98">
   <si>
     <t>A10137873</t>
   </si>
@@ -234,9 +234,6 @@
     <t>73.68</t>
   </si>
   <si>
-    <t>6.7f</t>
-  </si>
-  <si>
     <t>13010164</t>
   </si>
   <si>
@@ -270,12 +267,6 @@
     <t>Sherbrooke</t>
   </si>
   <si>
-    <t>1f</t>
-  </si>
-  <si>
-    <t>95.48</t>
-  </si>
-  <si>
     <t>AUTOMATION TRB SFA</t>
   </si>
   <si>
@@ -295,9 +286,6 @@
   </si>
   <si>
     <t>AutomationCKQ</t>
-  </si>
-  <si>
-    <t>84.87</t>
   </si>
   <si>
     <t>isFirstMaintenancetoEdit</t>
@@ -861,13 +849,13 @@
         <v>55</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="T1" s="8" t="s">
         <v>17</v>
@@ -891,10 +879,10 @@
         <v>59</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>5</v>
@@ -903,10 +891,10 @@
         <v>60</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>63</v>
@@ -915,10 +903,10 @@
         <v>64</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>36</v>
@@ -935,7 +923,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -971,7 +959,7 @@
         <v>58</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>54</v>
@@ -980,13 +968,13 @@
         <v>56</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="T2" s="9">
         <v>0</v>
@@ -1016,28 +1004,28 @@
         <v>65</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AE2" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AF2" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AH2" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AI2" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AJ2" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AK2" s="3" t="s">
         <v>40</v>
@@ -1174,13 +1162,13 @@
         <v>55</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="T1" s="8" t="s">
         <v>17</v>
@@ -1230,7 +1218,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C2" s="4">
         <v>1813</v>
@@ -1257,7 +1245,7 @@
         <v>13012004</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>7</v>
@@ -1275,13 +1263,13 @@
         <v>56</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="T2" s="9">
         <v>0</v>
@@ -1363,7 +1351,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1462,13 +1452,13 @@
         <v>55</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="W1" s="8" t="s">
         <v>17</v>
@@ -1518,7 +1508,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -1539,7 +1529,7 @@
         <v>47</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J2" s="4">
         <v>2</v>
@@ -1554,7 +1544,7 @@
         <v>46</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>7</v>
@@ -1563,7 +1553,7 @@
         <v>58</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>54</v>
@@ -1572,13 +1562,13 @@
         <v>56</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="W2" s="9">
         <v>0</v>
@@ -1599,19 +1589,19 @@
         <v>65</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="AE2" s="7" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="AF2" s="7" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>40</v>
@@ -1627,7 +1617,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="M2:N2 AF2:AG2 T2:V2" numberStoredAsText="1"/>
+    <ignoredError sqref="M2:N2 T2:V2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1694,7 +1684,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>39</v>
@@ -1765,7 +1755,7 @@
         <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1785,7 +1775,7 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>